<commit_message>
refs #848 Globale Klausel
Former-commit-id: 1a471134d05d9078c4d1605ac833a913126f4bc4
</commit_message>
<xml_diff>
--- a/doc/Bericht/05_Technischer Bericht/06_Hardware Evaluation & Tests/NutzwertmatrixMonitorkonstellationVideoWall.xlsx
+++ b/doc/Bericht/05_Technischer Bericht/06_Hardware Evaluation & Tests/NutzwertmatrixMonitorkonstellationVideoWall.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Variante 1</t>
   </si>
@@ -52,9 +52,6 @@
     <t>1 x 6 55" Monitore</t>
   </si>
   <si>
-    <t>Einbringung in Raumhöhe</t>
-  </si>
-  <si>
     <t>Bildschirmfläche überblickbar</t>
   </si>
   <si>
@@ -64,13 +61,19 @@
     <t>Darstellungsqualität/-grösse zum Lesen</t>
   </si>
   <si>
-    <t>Bemerkung: Die Gewichtungs- / Bewertungsskala geht von 1 (am schlechtesten) bis 5 (am besten).</t>
-  </si>
-  <si>
     <t>Durch die Nutzwertanalyse geht die Konstellation "Variante 1: 3 x 3 55" Monitore" als Sieger hervor.</t>
   </si>
   <si>
     <t>Nutzwertanalyse: Auswahl Monitorkonstellation für Video Wall</t>
+  </si>
+  <si>
+    <t>Bemerkung: Die Gewichtungs- / Bewertungsskala geht von wenig (1), bedingt (3) bis zu sehr wichtig (5).</t>
+  </si>
+  <si>
+    <t>Kosten</t>
+  </si>
+  <si>
+    <t>Einbringung in Raumhöhe (Raumgefühl)</t>
   </si>
 </sst>
 </file>
@@ -179,7 +182,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
@@ -197,6 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -516,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,48 +533,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="A1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="13" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="14"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="15" t="s">
+      <c r="F3" s="17"/>
+      <c r="G3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="16"/>
+      <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -600,7 +604,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -613,11 +617,11 @@
         <v>15</v>
       </c>
       <c r="E5" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="8">
         <f>B5*E5</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G5" s="7">
         <v>5</v>
@@ -629,36 +633,36 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="8">
-        <f t="shared" ref="D6:D8" si="0">B6*C6</f>
-        <v>12</v>
+        <f t="shared" ref="D6:D9" si="0">B6*C6</f>
+        <v>15</v>
       </c>
       <c r="E6" s="7">
         <v>5</v>
       </c>
       <c r="F6" s="8">
-        <f t="shared" ref="F6:F8" si="1">B6*E6</f>
+        <f t="shared" ref="F6:F9" si="1">B6*E6</f>
         <v>15</v>
       </c>
       <c r="G6" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H6" s="8">
-        <f t="shared" ref="H6:H8" si="2">B6*G6</f>
-        <v>6</v>
+        <f t="shared" ref="H6:H9" si="2">B6*G6</f>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -685,107 +689,136 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8">
+    <row r="8" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="11">
         <v>5</v>
       </c>
       <c r="C8" s="7">
         <v>5</v>
       </c>
       <c r="D8" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D8" si="3">B8*C8</f>
         <v>25</v>
       </c>
       <c r="E8" s="7">
         <v>3</v>
       </c>
       <c r="F8" s="8">
+        <f t="shared" ref="F8" si="4">B8*E8</f>
+        <v>15</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8">
+        <f t="shared" ref="H8" si="5">B8*G8</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>5</v>
+      </c>
+      <c r="F9" s="8">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="G8" s="7">
-        <v>2</v>
-      </c>
-      <c r="H8" s="8">
+        <v>5</v>
+      </c>
+      <c r="G9" s="7">
+        <v>3</v>
+      </c>
+      <c r="H9" s="8">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10">
-        <f>SUM(D5:D8)</f>
-        <v>57</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10">
-        <f>SUM(F5:F8)</f>
-        <v>45</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="10">
-        <f>SUM(H5:H8)</f>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="9"/>
       <c r="D10" s="10">
-        <f>IF(D9&gt;=F9,IF(D9&gt;=H9,1,2),IF(D9&gt;=H9,2,3))</f>
-        <v>1</v>
+        <f>SUM(D5:D9)</f>
+        <v>61</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="10">
-        <f>IF(F9&gt;=H9,IF(F9&gt;=D9,1,2),IF(F9&gt;=D9,2,3))</f>
-        <v>2</v>
+        <f>SUM(F5:F9)</f>
+        <v>45</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="10">
-        <f>IF(H9&gt;=D9,IF(H9&gt;=F9,1,2),IF(H9&gt;=F9,2,3))</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-    </row>
+        <f>SUM(H5:H9)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10">
+        <f>IF(D10&gt;=F10,IF(D10&gt;=H10,1,2),IF(D10&gt;=H10,2,3))</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10">
+        <f>IF(F10&gt;=H10,IF(F10&gt;=D10,1,2),IF(F10&gt;=D10,2,3))</f>
+        <v>2</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="10">
+        <f>IF(H10&gt;=D10,IF(H10&gt;=F10,1,2),IF(H10&gt;=F10,2,3))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A12:H12"/>
     <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A14:H14"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>

</xml_diff>